<commit_message>
docs: modified Test case
</commit_message>
<xml_diff>
--- a/artifacts/sogoing_test_case.xlsx
+++ b/artifacts/sogoing_test_case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangyeunpark/Desktop/UOS/3rd/2nd/Software-Engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangyeunpark/Desktop/UOS/3rd/2nd/Software-Engineering/Assignment/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F92E330-FA9C-4F40-8822-4F2AC3CD57A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECB84A-2343-C142-A21B-9AAB23C22BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9740" yWindow="740" windowWidth="19660" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="309">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -4714,13 +4714,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Use case # UC-010 (추가 예정)</t>
-  </si>
-  <si>
-    <t>Use case # UC-010 (추가 예정)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Use case # UC-009</t>
   </si>
   <si>
@@ -5622,6 +5615,10 @@
   </si>
   <si>
     <t>김고은, 석우진, 이강민, 정구홍, 조종빈</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use case # UC-010</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -6236,8 +6233,8 @@
   </sheetPr>
   <dimension ref="A1:AE1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="K51" zoomScale="50" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6409,7 +6406,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -6441,7 +6438,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -6479,7 +6476,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -7013,10 +7010,10 @@
         <v>38</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>21</v>
@@ -7718,7 +7715,7 @@
         <v>98</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>100</v>
@@ -7883,25 +7880,25 @@
         <v>196</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>241</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>21</v>
@@ -7939,19 +7936,19 @@
     <row r="33" spans="1:31" ht="133">
       <c r="A33" s="16"/>
       <c r="B33" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>41</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>243</v>
@@ -7998,10 +7995,10 @@
     <row r="34" spans="1:31" ht="152">
       <c r="A34" s="16"/>
       <c r="B34" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>42</v>
@@ -8010,7 +8007,7 @@
         <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>245</v>
@@ -8057,10 +8054,10 @@
     <row r="35" spans="1:31" ht="152">
       <c r="A35" s="16"/>
       <c r="B35" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>50</v>
@@ -8069,7 +8066,7 @@
         <v>46</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>247</v>
@@ -8116,19 +8113,19 @@
     <row r="36" spans="1:31" ht="85">
       <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>38</v>
@@ -8175,19 +8172,19 @@
     <row r="37" spans="1:31" ht="119">
       <c r="A37" s="16"/>
       <c r="B37" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D37" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>250</v>
@@ -8234,10 +8231,10 @@
     <row r="38" spans="1:31" ht="136">
       <c r="A38" s="16"/>
       <c r="B38" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>259</v>
@@ -8246,7 +8243,7 @@
         <v>56</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>250</v>
@@ -8742,7 +8739,7 @@
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1" t="s">
-        <v>265</v>
+        <v>308</v>
       </c>
       <c r="P46" s="17"/>
       <c r="Q46" s="5"/>
@@ -8800,7 +8797,7 @@
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1" t="s">
-        <v>265</v>
+        <v>308</v>
       </c>
       <c r="P47" s="17"/>
       <c r="Q47" s="5"/>
@@ -8858,7 +8855,7 @@
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="P48" s="17"/>
       <c r="Q48" s="5"/>
@@ -8916,7 +8913,7 @@
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P49" s="17"/>
       <c r="Q49" s="5"/>
@@ -8974,7 +8971,7 @@
       </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P50" s="17"/>
       <c r="Q50" s="5"/>
@@ -9032,7 +9029,7 @@
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P51" s="17"/>
       <c r="Q51" s="5"/>
@@ -9090,7 +9087,7 @@
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P52" s="17"/>
       <c r="Q52" s="5"/>
@@ -9148,7 +9145,7 @@
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="P53" s="17"/>
       <c r="Q53" s="5"/>
@@ -9206,7 +9203,7 @@
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1" t="s">
-        <v>264</v>
+        <v>308</v>
       </c>
       <c r="P54" s="17"/>
       <c r="Q54" s="5"/>
@@ -9264,7 +9261,7 @@
       </c>
       <c r="N55" s="1"/>
       <c r="O55" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P55" s="17"/>
       <c r="Q55" s="5"/>
@@ -9322,7 +9319,7 @@
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P56" s="17"/>
       <c r="Q56" s="5"/>
@@ -9380,7 +9377,7 @@
       </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P57" s="17"/>
       <c r="Q57" s="5"/>
@@ -9404,25 +9401,25 @@
         <v>216</v>
       </c>
       <c r="C58" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D58" s="25" t="s">
         <v>271</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>273</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>21</v>
@@ -9438,7 +9435,7 @@
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P58" s="17"/>
       <c r="Q58" s="5"/>
@@ -9462,16 +9459,16 @@
         <v>217</v>
       </c>
       <c r="C59" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>272</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>274</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>254</v>
@@ -9496,7 +9493,7 @@
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P59" s="17"/>
       <c r="Q59" s="5"/>
@@ -9520,16 +9517,16 @@
         <v>218</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>255</v>
@@ -9554,7 +9551,7 @@
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P60" s="17"/>
       <c r="Q60" s="5"/>
@@ -9578,16 +9575,16 @@
         <v>219</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>256</v>
@@ -9612,7 +9609,7 @@
       </c>
       <c r="N61" s="1"/>
       <c r="O61" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P61" s="17"/>
       <c r="Q61" s="5"/>
@@ -9670,7 +9667,7 @@
       </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="P62" s="17"/>
       <c r="Q62" s="5"/>
@@ -9728,7 +9725,7 @@
       </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P63" s="17"/>
       <c r="Q63" s="5"/>

</xml_diff>

<commit_message>
docs: modified test execution date
</commit_message>
<xml_diff>
--- a/artifacts/sogoing_test_case.xlsx
+++ b/artifacts/sogoing_test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangyeunpark/Desktop/UOS/3rd/2nd/Software-Engineering/Assignment/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FECB84A-2343-C142-A21B-9AAB23C22BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24F9CBA-327C-A94D-89A8-D4C37B235440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9740" yWindow="740" windowWidth="19660" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6233,8 +6233,8 @@
   </sheetPr>
   <dimension ref="A1:AE1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K51" zoomScale="50" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6482,7 +6482,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="24">
-        <v>45626</v>
+        <v>45634</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>

</xml_diff>

<commit_message>
docs: update Test case
</commit_message>
<xml_diff>
--- a/artifacts/sogoing_test_case.xlsx
+++ b/artifacts/sogoing_test_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangyeunpark/Desktop/UOS/3rd/2nd/Software-Engineering/Assignment/artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24F9CBA-327C-A94D-89A8-D4C37B235440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A03B3FA-6D04-F94D-851E-1052860FC651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="740" windowWidth="19660" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="311">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -5621,6 +5621,14 @@
     <t>Use case # UC-010</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>회원 정보 삭제 &amp; 모집 리스트 화면으로 이동. 
+그러나 회원 정보 삭제 시 종종 오류 발생.</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
 </sst>
 </file>
 
@@ -6233,8 +6241,8 @@
   </sheetPr>
   <dimension ref="A1:AE1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="143" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -9071,13 +9079,13 @@
         <v>149</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>149</v>
+        <v>309</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>20</v>
+        <v>310</v>
       </c>
       <c r="L52" s="1" t="s">
         <v>226</v>

</xml_diff>